<commit_message>
Fix sheet names in Questions 4.0
</commit_message>
<xml_diff>
--- a/Questions 2.0.xlsx
+++ b/Questions 2.0.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josephcampodonico/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josephcampodonico/Desktop/ADDM/CMPINF2100/Publish/CMPINF_2100_project/Leadership-Assessment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD2673A0-899E-C842-AFAA-B55300B71343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{778D0EF4-DBAE-DF4A-A868-A268DD55F109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{0E57FAF4-CDC2-49B6-BCD9-EBFD6CE9E32E}"/>
+    <workbookView xWindow="2120" yWindow="-20960" windowWidth="38400" windowHeight="21100" xr2:uid="{0E57FAF4-CDC2-49B6-BCD9-EBFD6CE9E32E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Questions" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -830,7 +830,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -838,9 +838,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1160,7 +1159,7 @@
   <dimension ref="A1:D474"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1168,7 +1167,6 @@
     <col min="1" max="1" width="8.6640625" style="1"/>
     <col min="2" max="2" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -1195,7 +1193,7 @@
       <c r="C2" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" t="s">
         <v>100</v>
       </c>
     </row>
@@ -1209,7 +1207,7 @@
       <c r="C3" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1223,7 +1221,7 @@
       <c r="C4" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1237,7 +1235,7 @@
       <c r="C5" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1251,7 +1249,7 @@
       <c r="C6" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1265,7 +1263,7 @@
       <c r="C7" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1279,7 +1277,7 @@
       <c r="C8" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" t="s">
         <v>120</v>
       </c>
     </row>
@@ -1293,7 +1291,7 @@
       <c r="C9" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1307,7 +1305,7 @@
       <c r="C10" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1321,7 +1319,7 @@
       <c r="C11" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1335,7 +1333,7 @@
       <c r="C12" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1349,7 +1347,7 @@
       <c r="C13" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1363,7 +1361,7 @@
       <c r="C14" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" t="s">
         <v>119</v>
       </c>
     </row>
@@ -1377,7 +1375,7 @@
       <c r="C15" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="4" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1391,7 +1389,7 @@
       <c r="C16" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="4" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1405,7 +1403,7 @@
       <c r="C17" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1419,7 +1417,7 @@
       <c r="C18" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="4" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1433,7 +1431,7 @@
       <c r="C19" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="4" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1447,7 +1445,7 @@
       <c r="C20" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" t="s">
         <v>118</v>
       </c>
     </row>
@@ -1461,7 +1459,7 @@
       <c r="C21" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="4" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1475,7 +1473,7 @@
       <c r="C22" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1489,7 +1487,7 @@
       <c r="C23" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="4" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1503,7 +1501,7 @@
       <c r="C24" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1517,7 +1515,7 @@
       <c r="C25" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1531,7 +1529,7 @@
       <c r="C26" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1545,7 +1543,7 @@
       <c r="C27" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="4" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1559,7 +1557,7 @@
       <c r="C28" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="4" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1573,7 +1571,7 @@
       <c r="C29" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="4" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1587,7 +1585,7 @@
       <c r="C30" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D30" s="4" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1601,7 +1599,7 @@
       <c r="C31" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D31" s="4" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1615,7 +1613,7 @@
       <c r="C32" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" t="s">
         <v>116</v>
       </c>
     </row>
@@ -1629,7 +1627,7 @@
       <c r="C33" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D33" s="4" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1643,7 +1641,7 @@
       <c r="C34" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D34" s="4" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1657,7 +1655,7 @@
       <c r="C35" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D35" s="4" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1671,7 +1669,7 @@
       <c r="C36" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D36" s="4" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1685,7 +1683,7 @@
       <c r="C37" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="D37" s="4" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1699,7 +1697,7 @@
       <c r="C38" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D38" t="s">
         <v>115</v>
       </c>
     </row>
@@ -1713,7 +1711,7 @@
       <c r="C39" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="D39" s="4" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1727,7 +1725,7 @@
       <c r="C40" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D40" s="5" t="s">
+      <c r="D40" s="4" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1741,7 +1739,7 @@
       <c r="C41" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="D41" s="4" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1755,7 +1753,7 @@
       <c r="C42" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D42" s="5" t="s">
+      <c r="D42" s="4" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1769,7 +1767,7 @@
       <c r="C43" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D43" s="5" t="s">
+      <c r="D43" s="4" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1783,7 +1781,7 @@
       <c r="C44" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D44" s="4" t="s">
+      <c r="D44" t="s">
         <v>114</v>
       </c>
     </row>
@@ -1797,7 +1795,7 @@
       <c r="C45" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D45" s="5" t="s">
+      <c r="D45" s="4" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1811,7 +1809,7 @@
       <c r="C46" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="D46" s="4" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1825,7 +1823,7 @@
       <c r="C47" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D47" s="5" t="s">
+      <c r="D47" s="4" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1839,7 +1837,7 @@
       <c r="C48" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D48" s="5" t="s">
+      <c r="D48" s="4" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1853,7 +1851,7 @@
       <c r="C49" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D49" s="5" t="s">
+      <c r="D49" s="4" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1867,7 +1865,7 @@
       <c r="C50" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D50" s="4" t="s">
+      <c r="D50" t="s">
         <v>113</v>
       </c>
     </row>
@@ -1881,7 +1879,7 @@
       <c r="C51" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D51" s="5" t="s">
+      <c r="D51" s="4" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1895,7 +1893,7 @@
       <c r="C52" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D52" s="5" t="s">
+      <c r="D52" s="4" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1909,7 +1907,7 @@
       <c r="C53" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D53" s="5" t="s">
+      <c r="D53" s="4" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1923,7 +1921,7 @@
       <c r="C54" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D54" s="5" t="s">
+      <c r="D54" s="4" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1937,7 +1935,7 @@
       <c r="C55" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D55" s="5" t="s">
+      <c r="D55" s="4" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1951,7 +1949,7 @@
       <c r="C56" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D56" s="4" t="s">
+      <c r="D56" t="s">
         <v>112</v>
       </c>
     </row>
@@ -1965,7 +1963,7 @@
       <c r="C57" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D57" s="5" t="s">
+      <c r="D57" s="4" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1979,7 +1977,7 @@
       <c r="C58" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D58" s="5" t="s">
+      <c r="D58" s="4" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1993,7 +1991,7 @@
       <c r="C59" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D59" s="5" t="s">
+      <c r="D59" s="4" t="s">
         <v>47</v>
       </c>
     </row>
@@ -2007,7 +2005,7 @@
       <c r="C60" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D60" s="5" t="s">
+      <c r="D60" s="4" t="s">
         <v>48</v>
       </c>
     </row>
@@ -2021,7 +2019,7 @@
       <c r="C61" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D61" s="5" t="s">
+      <c r="D61" s="4" t="s">
         <v>49</v>
       </c>
     </row>
@@ -2035,7 +2033,7 @@
       <c r="C62" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D62" s="4" t="s">
+      <c r="D62" t="s">
         <v>111</v>
       </c>
     </row>
@@ -2049,7 +2047,7 @@
       <c r="C63" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D63" s="5" t="s">
+      <c r="D63" s="4" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2063,7 +2061,7 @@
       <c r="C64" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D64" s="5" t="s">
+      <c r="D64" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2077,7 +2075,7 @@
       <c r="C65" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D65" s="5" t="s">
+      <c r="D65" s="4" t="s">
         <v>52</v>
       </c>
     </row>
@@ -2091,7 +2089,7 @@
       <c r="C66" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D66" s="5" t="s">
+      <c r="D66" s="4" t="s">
         <v>53</v>
       </c>
     </row>
@@ -2105,7 +2103,7 @@
       <c r="C67" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D67" s="5" t="s">
+      <c r="D67" s="4" t="s">
         <v>54</v>
       </c>
     </row>
@@ -2119,7 +2117,7 @@
       <c r="C68" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D68" s="4" t="s">
+      <c r="D68" t="s">
         <v>110</v>
       </c>
     </row>
@@ -2133,7 +2131,7 @@
       <c r="C69" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D69" s="5" t="s">
+      <c r="D69" s="4" t="s">
         <v>55</v>
       </c>
     </row>
@@ -2147,7 +2145,7 @@
       <c r="C70" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D70" s="5" t="s">
+      <c r="D70" s="4" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2161,7 +2159,7 @@
       <c r="C71" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D71" s="5" t="s">
+      <c r="D71" s="4" t="s">
         <v>57</v>
       </c>
     </row>
@@ -2175,7 +2173,7 @@
       <c r="C72" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D72" s="5" t="s">
+      <c r="D72" s="4" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2189,7 +2187,7 @@
       <c r="C73" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D73" s="5" t="s">
+      <c r="D73" s="4" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2203,7 +2201,7 @@
       <c r="C74" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D74" s="4" t="s">
+      <c r="D74" t="s">
         <v>109</v>
       </c>
     </row>
@@ -2217,7 +2215,7 @@
       <c r="C75" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D75" s="5" t="s">
+      <c r="D75" s="4" t="s">
         <v>60</v>
       </c>
     </row>
@@ -2231,7 +2229,7 @@
       <c r="C76" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D76" s="5" t="s">
+      <c r="D76" s="4" t="s">
         <v>61</v>
       </c>
     </row>
@@ -2245,7 +2243,7 @@
       <c r="C77" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D77" s="5" t="s">
+      <c r="D77" s="4" t="s">
         <v>62</v>
       </c>
     </row>
@@ -2259,7 +2257,7 @@
       <c r="C78" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D78" s="5" t="s">
+      <c r="D78" s="4" t="s">
         <v>63</v>
       </c>
     </row>
@@ -2273,7 +2271,7 @@
       <c r="C79" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D79" s="5" t="s">
+      <c r="D79" s="4" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2287,7 +2285,7 @@
       <c r="C80" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D80" s="4" t="s">
+      <c r="D80" t="s">
         <v>108</v>
       </c>
     </row>
@@ -2301,7 +2299,7 @@
       <c r="C81" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D81" s="5" t="s">
+      <c r="D81" s="4" t="s">
         <v>65</v>
       </c>
     </row>
@@ -2315,7 +2313,7 @@
       <c r="C82" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D82" s="5" t="s">
+      <c r="D82" s="4" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2329,7 +2327,7 @@
       <c r="C83" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D83" s="5" t="s">
+      <c r="D83" s="4" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2343,7 +2341,7 @@
       <c r="C84" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D84" s="5" t="s">
+      <c r="D84" s="4" t="s">
         <v>68</v>
       </c>
     </row>
@@ -2357,7 +2355,7 @@
       <c r="C85" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D85" s="5" t="s">
+      <c r="D85" s="4" t="s">
         <v>69</v>
       </c>
     </row>
@@ -2371,7 +2369,7 @@
       <c r="C86" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D86" s="4" t="s">
+      <c r="D86" t="s">
         <v>107</v>
       </c>
     </row>
@@ -2385,7 +2383,7 @@
       <c r="C87" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D87" s="5" t="s">
+      <c r="D87" s="4" t="s">
         <v>70</v>
       </c>
     </row>
@@ -2399,7 +2397,7 @@
       <c r="C88" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D88" s="5" t="s">
+      <c r="D88" s="4" t="s">
         <v>71</v>
       </c>
     </row>
@@ -2413,7 +2411,7 @@
       <c r="C89" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D89" s="5" t="s">
+      <c r="D89" s="4" t="s">
         <v>72</v>
       </c>
     </row>
@@ -2427,7 +2425,7 @@
       <c r="C90" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D90" s="5" t="s">
+      <c r="D90" s="4" t="s">
         <v>73</v>
       </c>
     </row>
@@ -2441,7 +2439,7 @@
       <c r="C91" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D91" s="5" t="s">
+      <c r="D91" s="4" t="s">
         <v>74</v>
       </c>
     </row>
@@ -2455,7 +2453,7 @@
       <c r="C92" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D92" s="4" t="s">
+      <c r="D92" t="s">
         <v>106</v>
       </c>
     </row>
@@ -2469,7 +2467,7 @@
       <c r="C93" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D93" s="5" t="s">
+      <c r="D93" s="4" t="s">
         <v>75</v>
       </c>
     </row>
@@ -2483,7 +2481,7 @@
       <c r="C94" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D94" s="5" t="s">
+      <c r="D94" s="4" t="s">
         <v>76</v>
       </c>
     </row>
@@ -2497,7 +2495,7 @@
       <c r="C95" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D95" s="5" t="s">
+      <c r="D95" s="4" t="s">
         <v>77</v>
       </c>
     </row>
@@ -2511,7 +2509,7 @@
       <c r="C96" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D96" s="5" t="s">
+      <c r="D96" s="4" t="s">
         <v>78</v>
       </c>
     </row>
@@ -2525,7 +2523,7 @@
       <c r="C97" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D97" s="5" t="s">
+      <c r="D97" s="4" t="s">
         <v>79</v>
       </c>
     </row>
@@ -2539,7 +2537,7 @@
       <c r="C98" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D98" s="4" t="s">
+      <c r="D98" t="s">
         <v>105</v>
       </c>
     </row>
@@ -2553,7 +2551,7 @@
       <c r="C99" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D99" s="5" t="s">
+      <c r="D99" s="4" t="s">
         <v>80</v>
       </c>
     </row>
@@ -2567,7 +2565,7 @@
       <c r="C100" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D100" s="5" t="s">
+      <c r="D100" s="4" t="s">
         <v>81</v>
       </c>
     </row>
@@ -2581,7 +2579,7 @@
       <c r="C101" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D101" s="5" t="s">
+      <c r="D101" s="4" t="s">
         <v>82</v>
       </c>
     </row>
@@ -2595,7 +2593,7 @@
       <c r="C102" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D102" s="5" t="s">
+      <c r="D102" s="4" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2609,7 +2607,7 @@
       <c r="C103" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D103" s="5" t="s">
+      <c r="D103" s="4" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2623,7 +2621,7 @@
       <c r="C104" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D104" s="4" t="s">
+      <c r="D104" t="s">
         <v>104</v>
       </c>
     </row>
@@ -2637,7 +2635,7 @@
       <c r="C105" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D105" s="5" t="s">
+      <c r="D105" s="4" t="s">
         <v>85</v>
       </c>
     </row>
@@ -2651,7 +2649,7 @@
       <c r="C106" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D106" s="5" t="s">
+      <c r="D106" s="4" t="s">
         <v>86</v>
       </c>
     </row>
@@ -2665,7 +2663,7 @@
       <c r="C107" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D107" s="5" t="s">
+      <c r="D107" s="4" t="s">
         <v>87</v>
       </c>
     </row>
@@ -2679,7 +2677,7 @@
       <c r="C108" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D108" s="5" t="s">
+      <c r="D108" s="4" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2693,7 +2691,7 @@
       <c r="C109" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D109" s="5" t="s">
+      <c r="D109" s="4" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2707,7 +2705,7 @@
       <c r="C110" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D110" s="4" t="s">
+      <c r="D110" t="s">
         <v>103</v>
       </c>
     </row>
@@ -2721,7 +2719,7 @@
       <c r="C111" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D111" s="5" t="s">
+      <c r="D111" s="4" t="s">
         <v>90</v>
       </c>
     </row>
@@ -2735,7 +2733,7 @@
       <c r="C112" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D112" s="5" t="s">
+      <c r="D112" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2749,7 +2747,7 @@
       <c r="C113" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D113" s="5" t="s">
+      <c r="D113" s="4" t="s">
         <v>92</v>
       </c>
     </row>
@@ -2763,7 +2761,7 @@
       <c r="C114" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D114" s="5" t="s">
+      <c r="D114" s="4" t="s">
         <v>93</v>
       </c>
     </row>
@@ -2777,7 +2775,7 @@
       <c r="C115" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D115" s="5" t="s">
+      <c r="D115" s="4" t="s">
         <v>94</v>
       </c>
     </row>
@@ -2791,7 +2789,7 @@
       <c r="C116" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D116" s="4" t="s">
+      <c r="D116" t="s">
         <v>102</v>
       </c>
     </row>
@@ -2805,7 +2803,7 @@
       <c r="C117" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D117" s="5" t="s">
+      <c r="D117" s="4" t="s">
         <v>95</v>
       </c>
     </row>
@@ -2819,7 +2817,7 @@
       <c r="C118" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D118" s="5" t="s">
+      <c r="D118" s="4" t="s">
         <v>96</v>
       </c>
     </row>
@@ -2833,7 +2831,7 @@
       <c r="C119" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D119" s="5" t="s">
+      <c r="D119" s="4" t="s">
         <v>97</v>
       </c>
     </row>
@@ -2847,7 +2845,7 @@
       <c r="C120" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D120" s="5" t="s">
+      <c r="D120" s="4" t="s">
         <v>98</v>
       </c>
     </row>
@@ -2861,7 +2859,7 @@
       <c r="C121" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D121" s="5" t="s">
+      <c r="D121" s="4" t="s">
         <v>99</v>
       </c>
     </row>
@@ -2875,7 +2873,7 @@
       <c r="C122" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D122" s="4" t="s">
+      <c r="D122" t="s">
         <v>218</v>
       </c>
     </row>
@@ -2889,7 +2887,7 @@
       <c r="C123" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D123" s="5" t="s">
+      <c r="D123" s="4" t="s">
         <v>121</v>
       </c>
     </row>
@@ -2903,7 +2901,7 @@
       <c r="C124" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D124" s="5" t="s">
+      <c r="D124" s="4" t="s">
         <v>122</v>
       </c>
     </row>
@@ -2917,7 +2915,7 @@
       <c r="C125" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D125" s="5" t="s">
+      <c r="D125" s="4" t="s">
         <v>123</v>
       </c>
     </row>
@@ -2931,7 +2929,7 @@
       <c r="C126" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D126" s="5" t="s">
+      <c r="D126" s="4" t="s">
         <v>124</v>
       </c>
     </row>
@@ -2945,7 +2943,7 @@
       <c r="C127" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D127" s="5" t="s">
+      <c r="D127" s="4" t="s">
         <v>125</v>
       </c>
     </row>
@@ -2959,7 +2957,7 @@
       <c r="C128" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D128" s="4" t="s">
+      <c r="D128" t="s">
         <v>219</v>
       </c>
     </row>
@@ -2973,7 +2971,7 @@
       <c r="C129" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D129" s="5" t="s">
+      <c r="D129" s="4" t="s">
         <v>126</v>
       </c>
     </row>
@@ -2987,7 +2985,7 @@
       <c r="C130" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D130" s="5" t="s">
+      <c r="D130" s="4" t="s">
         <v>127</v>
       </c>
     </row>
@@ -3001,7 +2999,7 @@
       <c r="C131" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D131" s="4" t="s">
+      <c r="D131" t="s">
         <v>220</v>
       </c>
     </row>
@@ -3015,7 +3013,7 @@
       <c r="C132" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D132" s="5" t="s">
+      <c r="D132" s="4" t="s">
         <v>128</v>
       </c>
     </row>
@@ -3029,7 +3027,7 @@
       <c r="C133" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D133" s="5" t="s">
+      <c r="D133" s="4" t="s">
         <v>129</v>
       </c>
     </row>
@@ -3043,7 +3041,7 @@
       <c r="C134" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D134" s="5" t="s">
+      <c r="D134" s="4" t="s">
         <v>130</v>
       </c>
     </row>
@@ -3057,7 +3055,7 @@
       <c r="C135" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D135" s="5" t="s">
+      <c r="D135" s="4" t="s">
         <v>131</v>
       </c>
     </row>
@@ -3071,7 +3069,7 @@
       <c r="C136" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D136" s="5" t="s">
+      <c r="D136" s="4" t="s">
         <v>132</v>
       </c>
     </row>
@@ -3085,7 +3083,7 @@
       <c r="C137" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D137" s="4" t="s">
+      <c r="D137" t="s">
         <v>221</v>
       </c>
     </row>
@@ -3099,7 +3097,7 @@
       <c r="C138" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D138" s="5" t="s">
+      <c r="D138" s="4" t="s">
         <v>133</v>
       </c>
     </row>
@@ -3113,7 +3111,7 @@
       <c r="C139" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D139" s="5" t="s">
+      <c r="D139" s="4" t="s">
         <v>134</v>
       </c>
     </row>
@@ -3127,7 +3125,7 @@
       <c r="C140" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D140" s="5" t="s">
+      <c r="D140" s="4" t="s">
         <v>135</v>
       </c>
     </row>
@@ -3141,7 +3139,7 @@
       <c r="C141" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D141" s="5" t="s">
+      <c r="D141" s="4" t="s">
         <v>136</v>
       </c>
     </row>
@@ -3155,7 +3153,7 @@
       <c r="C142" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D142" s="5" t="s">
+      <c r="D142" s="4" t="s">
         <v>137</v>
       </c>
     </row>
@@ -3169,7 +3167,7 @@
       <c r="C143" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D143" s="4" t="s">
+      <c r="D143" t="s">
         <v>222</v>
       </c>
     </row>
@@ -3183,7 +3181,7 @@
       <c r="C144" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D144" s="5" t="s">
+      <c r="D144" s="4" t="s">
         <v>138</v>
       </c>
     </row>
@@ -3197,7 +3195,7 @@
       <c r="C145" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D145" s="5" t="s">
+      <c r="D145" s="4" t="s">
         <v>139</v>
       </c>
     </row>
@@ -3211,7 +3209,7 @@
       <c r="C146" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D146" s="5" t="s">
+      <c r="D146" s="4" t="s">
         <v>140</v>
       </c>
     </row>
@@ -3225,7 +3223,7 @@
       <c r="C147" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D147" s="5" t="s">
+      <c r="D147" s="4" t="s">
         <v>141</v>
       </c>
     </row>
@@ -3239,7 +3237,7 @@
       <c r="C148" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D148" s="5" t="s">
+      <c r="D148" s="4" t="s">
         <v>142</v>
       </c>
     </row>
@@ -3253,7 +3251,7 @@
       <c r="C149" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D149" s="4" t="s">
+      <c r="D149" t="s">
         <v>223</v>
       </c>
     </row>
@@ -3267,7 +3265,7 @@
       <c r="C150" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D150" s="5" t="s">
+      <c r="D150" s="4" t="s">
         <v>143</v>
       </c>
     </row>
@@ -3281,7 +3279,7 @@
       <c r="C151" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D151" s="5" t="s">
+      <c r="D151" s="4" t="s">
         <v>144</v>
       </c>
     </row>
@@ -3295,7 +3293,7 @@
       <c r="C152" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D152" s="5" t="s">
+      <c r="D152" s="4" t="s">
         <v>145</v>
       </c>
     </row>
@@ -3309,7 +3307,7 @@
       <c r="C153" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D153" s="5" t="s">
+      <c r="D153" s="4" t="s">
         <v>146</v>
       </c>
     </row>
@@ -3323,7 +3321,7 @@
       <c r="C154" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D154" s="5" t="s">
+      <c r="D154" s="4" t="s">
         <v>147</v>
       </c>
     </row>
@@ -3337,7 +3335,7 @@
       <c r="C155" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D155" s="4" t="s">
+      <c r="D155" t="s">
         <v>224</v>
       </c>
     </row>
@@ -3351,7 +3349,7 @@
       <c r="C156" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D156" s="5" t="s">
+      <c r="D156" s="4" t="s">
         <v>148</v>
       </c>
     </row>
@@ -3365,7 +3363,7 @@
       <c r="C157" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D157" s="5" t="s">
+      <c r="D157" s="4" t="s">
         <v>149</v>
       </c>
     </row>
@@ -3379,7 +3377,7 @@
       <c r="C158" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D158" s="5" t="s">
+      <c r="D158" s="4" t="s">
         <v>150</v>
       </c>
     </row>
@@ -3393,7 +3391,7 @@
       <c r="C159" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D159" s="5" t="s">
+      <c r="D159" s="4" t="s">
         <v>151</v>
       </c>
     </row>
@@ -3407,7 +3405,7 @@
       <c r="C160" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D160" s="5" t="s">
+      <c r="D160" s="4" t="s">
         <v>152</v>
       </c>
     </row>
@@ -3421,7 +3419,7 @@
       <c r="C161" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D161" s="4" t="s">
+      <c r="D161" t="s">
         <v>225</v>
       </c>
     </row>
@@ -3435,7 +3433,7 @@
       <c r="C162" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D162" s="5" t="s">
+      <c r="D162" s="4" t="s">
         <v>153</v>
       </c>
     </row>
@@ -3449,7 +3447,7 @@
       <c r="C163" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D163" s="5" t="s">
+      <c r="D163" s="4" t="s">
         <v>154</v>
       </c>
     </row>
@@ -3463,7 +3461,7 @@
       <c r="C164" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D164" s="5" t="s">
+      <c r="D164" s="4" t="s">
         <v>155</v>
       </c>
     </row>
@@ -3477,7 +3475,7 @@
       <c r="C165" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D165" s="5" t="s">
+      <c r="D165" s="4" t="s">
         <v>156</v>
       </c>
     </row>
@@ -3491,7 +3489,7 @@
       <c r="C166" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D166" s="5" t="s">
+      <c r="D166" s="4" t="s">
         <v>157</v>
       </c>
     </row>
@@ -3505,7 +3503,7 @@
       <c r="C167" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D167" s="4" t="s">
+      <c r="D167" t="s">
         <v>226</v>
       </c>
     </row>
@@ -3519,7 +3517,7 @@
       <c r="C168" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D168" s="5" t="s">
+      <c r="D168" s="4" t="s">
         <v>158</v>
       </c>
     </row>
@@ -3533,7 +3531,7 @@
       <c r="C169" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D169" s="5" t="s">
+      <c r="D169" s="4" t="s">
         <v>159</v>
       </c>
     </row>
@@ -3547,7 +3545,7 @@
       <c r="C170" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D170" s="5" t="s">
+      <c r="D170" s="4" t="s">
         <v>160</v>
       </c>
     </row>
@@ -3561,7 +3559,7 @@
       <c r="C171" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D171" s="5" t="s">
+      <c r="D171" s="4" t="s">
         <v>161</v>
       </c>
     </row>
@@ -3575,7 +3573,7 @@
       <c r="C172" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D172" s="5" t="s">
+      <c r="D172" s="4" t="s">
         <v>162</v>
       </c>
     </row>
@@ -3589,7 +3587,7 @@
       <c r="C173" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D173" s="4" t="s">
+      <c r="D173" t="s">
         <v>227</v>
       </c>
     </row>
@@ -3603,7 +3601,7 @@
       <c r="C174" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D174" s="5" t="s">
+      <c r="D174" s="4" t="s">
         <v>163</v>
       </c>
     </row>
@@ -3617,7 +3615,7 @@
       <c r="C175" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D175" s="5" t="s">
+      <c r="D175" s="4" t="s">
         <v>164</v>
       </c>
     </row>
@@ -3631,7 +3629,7 @@
       <c r="C176" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D176" s="5" t="s">
+      <c r="D176" s="4" t="s">
         <v>165</v>
       </c>
     </row>
@@ -3645,7 +3643,7 @@
       <c r="C177" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D177" s="5" t="s">
+      <c r="D177" s="4" t="s">
         <v>166</v>
       </c>
     </row>
@@ -3659,7 +3657,7 @@
       <c r="C178" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D178" s="5" t="s">
+      <c r="D178" s="4" t="s">
         <v>167</v>
       </c>
     </row>
@@ -3673,7 +3671,7 @@
       <c r="C179" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D179" s="4" t="s">
+      <c r="D179" t="s">
         <v>228</v>
       </c>
     </row>
@@ -3687,7 +3685,7 @@
       <c r="C180" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D180" s="5" t="s">
+      <c r="D180" s="4" t="s">
         <v>168</v>
       </c>
     </row>
@@ -3701,7 +3699,7 @@
       <c r="C181" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D181" s="5" t="s">
+      <c r="D181" s="4" t="s">
         <v>169</v>
       </c>
     </row>
@@ -3715,7 +3713,7 @@
       <c r="C182" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D182" s="5" t="s">
+      <c r="D182" s="4" t="s">
         <v>170</v>
       </c>
     </row>
@@ -3729,7 +3727,7 @@
       <c r="C183" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D183" s="5" t="s">
+      <c r="D183" s="4" t="s">
         <v>171</v>
       </c>
     </row>
@@ -3743,7 +3741,7 @@
       <c r="C184" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D184" s="5" t="s">
+      <c r="D184" s="4" t="s">
         <v>172</v>
       </c>
     </row>
@@ -3757,7 +3755,7 @@
       <c r="C185" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D185" s="4" t="s">
+      <c r="D185" t="s">
         <v>229</v>
       </c>
     </row>
@@ -3771,7 +3769,7 @@
       <c r="C186" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D186" s="5" t="s">
+      <c r="D186" s="4" t="s">
         <v>173</v>
       </c>
     </row>
@@ -3785,7 +3783,7 @@
       <c r="C187" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D187" s="5" t="s">
+      <c r="D187" s="4" t="s">
         <v>174</v>
       </c>
     </row>
@@ -3799,7 +3797,7 @@
       <c r="C188" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D188" s="5" t="s">
+      <c r="D188" s="4" t="s">
         <v>175</v>
       </c>
     </row>
@@ -3813,7 +3811,7 @@
       <c r="C189" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D189" s="5" t="s">
+      <c r="D189" s="4" t="s">
         <v>176</v>
       </c>
     </row>
@@ -3827,7 +3825,7 @@
       <c r="C190" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D190" s="5" t="s">
+      <c r="D190" s="4" t="s">
         <v>177</v>
       </c>
     </row>
@@ -3841,7 +3839,7 @@
       <c r="C191" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D191" s="4" t="s">
+      <c r="D191" t="s">
         <v>230</v>
       </c>
     </row>
@@ -3855,7 +3853,7 @@
       <c r="C192" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D192" s="5" t="s">
+      <c r="D192" s="4" t="s">
         <v>178</v>
       </c>
     </row>
@@ -3869,7 +3867,7 @@
       <c r="C193" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D193" s="5" t="s">
+      <c r="D193" s="4" t="s">
         <v>179</v>
       </c>
     </row>
@@ -3883,7 +3881,7 @@
       <c r="C194" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D194" s="5" t="s">
+      <c r="D194" s="4" t="s">
         <v>180</v>
       </c>
     </row>
@@ -3897,7 +3895,7 @@
       <c r="C195" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D195" s="5" t="s">
+      <c r="D195" s="4" t="s">
         <v>181</v>
       </c>
     </row>
@@ -3911,7 +3909,7 @@
       <c r="C196" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D196" s="5" t="s">
+      <c r="D196" s="4" t="s">
         <v>182</v>
       </c>
     </row>
@@ -3925,7 +3923,7 @@
       <c r="C197" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D197" s="4" t="s">
+      <c r="D197" t="s">
         <v>231</v>
       </c>
     </row>
@@ -3939,7 +3937,7 @@
       <c r="C198" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D198" s="5" t="s">
+      <c r="D198" s="4" t="s">
         <v>183</v>
       </c>
     </row>
@@ -3953,7 +3951,7 @@
       <c r="C199" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D199" s="5" t="s">
+      <c r="D199" s="4" t="s">
         <v>184</v>
       </c>
     </row>
@@ -3967,7 +3965,7 @@
       <c r="C200" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D200" s="5" t="s">
+      <c r="D200" s="4" t="s">
         <v>185</v>
       </c>
     </row>
@@ -3981,7 +3979,7 @@
       <c r="C201" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D201" s="5" t="s">
+      <c r="D201" s="4" t="s">
         <v>186</v>
       </c>
     </row>
@@ -3995,7 +3993,7 @@
       <c r="C202" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D202" s="5" t="s">
+      <c r="D202" s="4" t="s">
         <v>187</v>
       </c>
     </row>
@@ -4009,7 +4007,7 @@
       <c r="C203" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D203" s="4" t="s">
+      <c r="D203" t="s">
         <v>232</v>
       </c>
     </row>
@@ -4023,7 +4021,7 @@
       <c r="C204" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D204" s="5" t="s">
+      <c r="D204" s="4" t="s">
         <v>188</v>
       </c>
     </row>
@@ -4037,7 +4035,7 @@
       <c r="C205" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D205" s="5" t="s">
+      <c r="D205" s="4" t="s">
         <v>189</v>
       </c>
     </row>
@@ -4051,7 +4049,7 @@
       <c r="C206" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D206" s="5" t="s">
+      <c r="D206" s="4" t="s">
         <v>190</v>
       </c>
     </row>
@@ -4065,7 +4063,7 @@
       <c r="C207" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D207" s="5" t="s">
+      <c r="D207" s="4" t="s">
         <v>191</v>
       </c>
     </row>
@@ -4079,7 +4077,7 @@
       <c r="C208" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D208" s="5" t="s">
+      <c r="D208" s="4" t="s">
         <v>192</v>
       </c>
     </row>
@@ -4093,7 +4091,7 @@
       <c r="C209" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D209" s="4" t="s">
+      <c r="D209" t="s">
         <v>233</v>
       </c>
     </row>
@@ -4107,7 +4105,7 @@
       <c r="C210" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D210" s="5" t="s">
+      <c r="D210" s="4" t="s">
         <v>193</v>
       </c>
     </row>
@@ -4121,7 +4119,7 @@
       <c r="C211" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D211" s="5" t="s">
+      <c r="D211" s="4" t="s">
         <v>194</v>
       </c>
     </row>
@@ -4135,7 +4133,7 @@
       <c r="C212" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D212" s="5" t="s">
+      <c r="D212" s="4" t="s">
         <v>195</v>
       </c>
     </row>
@@ -4149,7 +4147,7 @@
       <c r="C213" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D213" s="5" t="s">
+      <c r="D213" s="4" t="s">
         <v>196</v>
       </c>
     </row>
@@ -4163,7 +4161,7 @@
       <c r="C214" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D214" s="5" t="s">
+      <c r="D214" s="4" t="s">
         <v>197</v>
       </c>
     </row>
@@ -4177,7 +4175,7 @@
       <c r="C215" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D215" s="4" t="s">
+      <c r="D215" t="s">
         <v>234</v>
       </c>
     </row>
@@ -4191,7 +4189,7 @@
       <c r="C216" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D216" s="5" t="s">
+      <c r="D216" s="4" t="s">
         <v>198</v>
       </c>
     </row>
@@ -4205,7 +4203,7 @@
       <c r="C217" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D217" s="5" t="s">
+      <c r="D217" s="4" t="s">
         <v>199</v>
       </c>
     </row>
@@ -4219,7 +4217,7 @@
       <c r="C218" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D218" s="5" t="s">
+      <c r="D218" s="4" t="s">
         <v>200</v>
       </c>
     </row>
@@ -4233,7 +4231,7 @@
       <c r="C219" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D219" s="5" t="s">
+      <c r="D219" s="4" t="s">
         <v>201</v>
       </c>
     </row>
@@ -4247,7 +4245,7 @@
       <c r="C220" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D220" s="5" t="s">
+      <c r="D220" s="4" t="s">
         <v>202</v>
       </c>
     </row>
@@ -4261,7 +4259,7 @@
       <c r="C221" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D221" s="4" t="s">
+      <c r="D221" t="s">
         <v>235</v>
       </c>
     </row>
@@ -4275,7 +4273,7 @@
       <c r="C222" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D222" s="5" t="s">
+      <c r="D222" s="4" t="s">
         <v>203</v>
       </c>
     </row>
@@ -4289,7 +4287,7 @@
       <c r="C223" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D223" s="5" t="s">
+      <c r="D223" s="4" t="s">
         <v>204</v>
       </c>
     </row>
@@ -4303,7 +4301,7 @@
       <c r="C224" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D224" s="5" t="s">
+      <c r="D224" s="4" t="s">
         <v>205</v>
       </c>
     </row>
@@ -4317,7 +4315,7 @@
       <c r="C225" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D225" s="5" t="s">
+      <c r="D225" s="4" t="s">
         <v>206</v>
       </c>
     </row>
@@ -4331,7 +4329,7 @@
       <c r="C226" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D226" s="5" t="s">
+      <c r="D226" s="4" t="s">
         <v>207</v>
       </c>
     </row>
@@ -4345,7 +4343,7 @@
       <c r="C227" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D227" s="4" t="s">
+      <c r="D227" t="s">
         <v>236</v>
       </c>
     </row>
@@ -4359,7 +4357,7 @@
       <c r="C228" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D228" s="5" t="s">
+      <c r="D228" s="4" t="s">
         <v>208</v>
       </c>
     </row>
@@ -4373,7 +4371,7 @@
       <c r="C229" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D229" s="5" t="s">
+      <c r="D229" s="4" t="s">
         <v>209</v>
       </c>
     </row>
@@ -4387,7 +4385,7 @@
       <c r="C230" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D230" s="5" t="s">
+      <c r="D230" s="4" t="s">
         <v>210</v>
       </c>
     </row>
@@ -4401,7 +4399,7 @@
       <c r="C231" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D231" s="5" t="s">
+      <c r="D231" s="4" t="s">
         <v>211</v>
       </c>
     </row>
@@ -4415,7 +4413,7 @@
       <c r="C232" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D232" s="5" t="s">
+      <c r="D232" s="4" t="s">
         <v>212</v>
       </c>
     </row>
@@ -4429,7 +4427,7 @@
       <c r="C233" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D233" s="4" t="s">
+      <c r="D233" t="s">
         <v>237</v>
       </c>
     </row>
@@ -4443,7 +4441,7 @@
       <c r="C234" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D234" s="5" t="s">
+      <c r="D234" s="4" t="s">
         <v>213</v>
       </c>
     </row>
@@ -4457,7 +4455,7 @@
       <c r="C235" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D235" s="5" t="s">
+      <c r="D235" s="4" t="s">
         <v>214</v>
       </c>
     </row>
@@ -4471,7 +4469,7 @@
       <c r="C236" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D236" s="5" t="s">
+      <c r="D236" s="4" t="s">
         <v>215</v>
       </c>
     </row>
@@ -4485,7 +4483,7 @@
       <c r="C237" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D237" s="5" t="s">
+      <c r="D237" s="4" t="s">
         <v>216</v>
       </c>
     </row>
@@ -4499,7 +4497,7 @@
       <c r="C238" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D238" s="5" t="s">
+      <c r="D238" s="4" t="s">
         <v>217</v>
       </c>
     </row>
@@ -4508,1176 +4506,240 @@
         <v>101</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A241"/>
-      <c r="B241"/>
-      <c r="C241"/>
-    </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A242"/>
-      <c r="B242"/>
-      <c r="C242"/>
-    </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A243"/>
-      <c r="B243"/>
-      <c r="C243"/>
-    </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A244"/>
-      <c r="B244"/>
-      <c r="C244"/>
-    </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A245"/>
-      <c r="B245"/>
-      <c r="C245"/>
-    </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A246"/>
-      <c r="B246"/>
-      <c r="C246"/>
-    </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A247"/>
-      <c r="B247"/>
-      <c r="C247"/>
-    </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A248"/>
-      <c r="B248"/>
-      <c r="C248"/>
-    </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A249"/>
-      <c r="B249"/>
-      <c r="C249"/>
-    </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A250"/>
-      <c r="B250"/>
-      <c r="C250"/>
-    </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A251"/>
-      <c r="B251"/>
-      <c r="C251"/>
-    </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A252"/>
-      <c r="B252"/>
-      <c r="C252"/>
-    </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A253"/>
-      <c r="B253"/>
-      <c r="C253"/>
-    </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A254"/>
-      <c r="B254"/>
-      <c r="C254"/>
-    </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A255"/>
-      <c r="B255"/>
-      <c r="C255"/>
-    </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A256"/>
-      <c r="B256"/>
-      <c r="C256"/>
-    </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A257"/>
-      <c r="B257"/>
-      <c r="C257"/>
-    </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A258"/>
-      <c r="B258"/>
-      <c r="C258"/>
-    </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A259"/>
-      <c r="B259"/>
-      <c r="C259"/>
-    </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A260"/>
-      <c r="B260"/>
-      <c r="C260"/>
-    </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A261"/>
-      <c r="B261"/>
-      <c r="C261"/>
-    </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A262"/>
-      <c r="B262"/>
-      <c r="C262"/>
-    </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A263"/>
-      <c r="B263"/>
-      <c r="C263"/>
-    </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A264"/>
-      <c r="B264"/>
-      <c r="C264"/>
-    </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A265"/>
-      <c r="B265"/>
-      <c r="C265"/>
-    </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A266"/>
-      <c r="B266"/>
-      <c r="C266"/>
-    </row>
-    <row r="267" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A267"/>
-      <c r="B267"/>
-      <c r="C267"/>
-    </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A268"/>
-      <c r="B268"/>
-      <c r="C268"/>
-    </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A269"/>
-      <c r="B269"/>
-      <c r="C269"/>
-    </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A270"/>
-      <c r="B270"/>
-      <c r="C270"/>
-    </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A271"/>
-      <c r="B271"/>
-      <c r="C271"/>
-    </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A272"/>
-      <c r="B272"/>
-      <c r="C272"/>
-    </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A273"/>
-      <c r="B273"/>
-      <c r="C273"/>
-    </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A274"/>
-      <c r="B274"/>
-      <c r="C274"/>
-    </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A275"/>
-      <c r="B275"/>
-      <c r="C275"/>
-    </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A276"/>
-      <c r="B276"/>
-      <c r="C276"/>
-    </row>
-    <row r="277" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A277"/>
-      <c r="B277"/>
-      <c r="C277"/>
-    </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A278"/>
-      <c r="B278"/>
-      <c r="C278"/>
-    </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A279"/>
-      <c r="B279"/>
-      <c r="C279"/>
-    </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A280"/>
-      <c r="B280"/>
-      <c r="C280"/>
-    </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A281"/>
-      <c r="B281"/>
-      <c r="C281"/>
-    </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A282"/>
-      <c r="B282"/>
-      <c r="C282"/>
-    </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A283"/>
-      <c r="B283"/>
-      <c r="C283"/>
-    </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A284"/>
-      <c r="B284"/>
-      <c r="C284"/>
-    </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A285"/>
-      <c r="B285"/>
-      <c r="C285"/>
-    </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A286"/>
-      <c r="B286"/>
-      <c r="C286"/>
-    </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A287"/>
-      <c r="B287"/>
-      <c r="C287"/>
-    </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A288"/>
-      <c r="B288"/>
-      <c r="C288"/>
-    </row>
-    <row r="289" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A289"/>
-      <c r="B289"/>
-      <c r="C289"/>
-    </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A290"/>
-      <c r="B290"/>
-      <c r="C290"/>
-    </row>
-    <row r="291" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A291"/>
-      <c r="B291"/>
-      <c r="C291"/>
-    </row>
-    <row r="292" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A292"/>
-      <c r="B292"/>
-      <c r="C292"/>
-    </row>
-    <row r="293" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A293"/>
-      <c r="B293"/>
-      <c r="C293"/>
-    </row>
-    <row r="294" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A294"/>
-      <c r="B294"/>
-      <c r="C294"/>
-    </row>
-    <row r="295" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A295"/>
-      <c r="B295"/>
-      <c r="C295"/>
-    </row>
-    <row r="296" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A296"/>
-      <c r="B296"/>
-      <c r="C296"/>
-    </row>
-    <row r="297" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A297"/>
-      <c r="B297"/>
-      <c r="C297"/>
-    </row>
-    <row r="298" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A298"/>
-      <c r="B298"/>
-      <c r="C298"/>
-    </row>
-    <row r="299" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A299"/>
-      <c r="B299"/>
-      <c r="C299"/>
-    </row>
-    <row r="300" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A300"/>
-      <c r="B300"/>
-      <c r="C300"/>
-    </row>
-    <row r="301" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A301"/>
-      <c r="B301"/>
-      <c r="C301"/>
-    </row>
-    <row r="302" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A302"/>
-      <c r="B302"/>
-      <c r="C302"/>
-    </row>
-    <row r="303" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A303"/>
-      <c r="B303"/>
-      <c r="C303"/>
-    </row>
-    <row r="304" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A304"/>
-      <c r="B304"/>
-      <c r="C304"/>
-    </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A305"/>
-      <c r="B305"/>
-      <c r="C305"/>
-    </row>
-    <row r="306" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A306"/>
-      <c r="B306"/>
-      <c r="C306"/>
-    </row>
-    <row r="307" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A307"/>
-      <c r="B307"/>
-      <c r="C307"/>
-    </row>
-    <row r="308" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A308"/>
-      <c r="B308"/>
-      <c r="C308"/>
-    </row>
-    <row r="309" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A309"/>
-      <c r="B309"/>
-      <c r="C309"/>
-    </row>
-    <row r="310" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A310"/>
-      <c r="B310"/>
-      <c r="C310"/>
-    </row>
-    <row r="311" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A311"/>
-      <c r="B311"/>
-      <c r="C311"/>
-    </row>
-    <row r="312" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A312"/>
-      <c r="B312"/>
-      <c r="C312"/>
-    </row>
-    <row r="313" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A313"/>
-      <c r="B313"/>
-      <c r="C313"/>
-    </row>
-    <row r="314" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A314"/>
-      <c r="B314"/>
-      <c r="C314"/>
-    </row>
-    <row r="315" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A315"/>
-      <c r="B315"/>
-      <c r="C315"/>
-    </row>
-    <row r="316" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A316"/>
-      <c r="B316"/>
-      <c r="C316"/>
-    </row>
-    <row r="317" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A317"/>
-      <c r="B317"/>
-      <c r="C317"/>
-    </row>
-    <row r="318" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A318"/>
-      <c r="B318"/>
-      <c r="C318"/>
-    </row>
-    <row r="319" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A319"/>
-      <c r="B319"/>
-      <c r="C319"/>
-    </row>
-    <row r="320" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A320"/>
-      <c r="B320"/>
-      <c r="C320"/>
-    </row>
-    <row r="321" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A321"/>
-      <c r="B321"/>
-      <c r="C321"/>
-    </row>
-    <row r="322" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A322"/>
-      <c r="B322"/>
-      <c r="C322"/>
-    </row>
-    <row r="323" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A323"/>
-      <c r="B323"/>
-      <c r="C323"/>
-    </row>
-    <row r="324" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A324"/>
-      <c r="B324"/>
-      <c r="C324"/>
-    </row>
-    <row r="325" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A325"/>
-      <c r="B325"/>
-      <c r="C325"/>
-    </row>
-    <row r="326" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A326"/>
-      <c r="B326"/>
-      <c r="C326"/>
-    </row>
-    <row r="327" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A327"/>
-      <c r="B327"/>
-      <c r="C327"/>
-    </row>
-    <row r="328" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A328"/>
-      <c r="B328"/>
-      <c r="C328"/>
-    </row>
-    <row r="329" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A329"/>
-      <c r="B329"/>
-      <c r="C329"/>
-    </row>
-    <row r="330" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A330"/>
-      <c r="B330"/>
-      <c r="C330"/>
-    </row>
-    <row r="331" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A331"/>
-      <c r="B331"/>
-      <c r="C331"/>
-    </row>
-    <row r="332" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A332"/>
-      <c r="B332"/>
-      <c r="C332"/>
-    </row>
-    <row r="333" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A333"/>
-      <c r="B333"/>
-      <c r="C333"/>
-    </row>
-    <row r="334" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A334"/>
-      <c r="B334"/>
-      <c r="C334"/>
-    </row>
-    <row r="335" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A335"/>
-      <c r="B335"/>
-      <c r="C335"/>
-    </row>
-    <row r="336" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A336"/>
-      <c r="B336"/>
-      <c r="C336"/>
-    </row>
-    <row r="337" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A337"/>
-      <c r="B337"/>
-      <c r="C337"/>
-    </row>
-    <row r="338" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A338"/>
-      <c r="B338"/>
-      <c r="C338"/>
-    </row>
-    <row r="339" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A339"/>
-      <c r="B339"/>
-      <c r="C339"/>
-    </row>
-    <row r="340" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A340"/>
-      <c r="B340"/>
-      <c r="C340"/>
-    </row>
-    <row r="341" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A341"/>
-      <c r="B341"/>
-      <c r="C341"/>
-    </row>
-    <row r="342" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A342"/>
-      <c r="B342"/>
-      <c r="C342"/>
-    </row>
-    <row r="343" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A343"/>
-      <c r="B343"/>
-      <c r="C343"/>
-    </row>
-    <row r="344" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A344"/>
-      <c r="B344"/>
-      <c r="C344"/>
-    </row>
-    <row r="345" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A345"/>
-      <c r="B345"/>
-      <c r="C345"/>
-    </row>
-    <row r="346" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A346"/>
-      <c r="B346"/>
-      <c r="C346"/>
-    </row>
-    <row r="347" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A347"/>
-      <c r="B347"/>
-      <c r="C347"/>
-    </row>
-    <row r="348" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A348"/>
-      <c r="B348"/>
-      <c r="C348"/>
-    </row>
-    <row r="349" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A349"/>
-      <c r="B349"/>
-      <c r="C349"/>
-    </row>
-    <row r="350" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A350"/>
-      <c r="B350"/>
-      <c r="C350"/>
-    </row>
-    <row r="351" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A351"/>
-      <c r="B351"/>
-      <c r="C351"/>
-    </row>
-    <row r="352" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A352"/>
-      <c r="B352"/>
-      <c r="C352"/>
-    </row>
-    <row r="353" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A353"/>
-      <c r="B353"/>
-      <c r="C353"/>
-    </row>
-    <row r="354" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A354"/>
-      <c r="B354"/>
-      <c r="C354"/>
-    </row>
-    <row r="355" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A355"/>
-      <c r="B355"/>
-      <c r="C355"/>
-    </row>
-    <row r="356" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A356"/>
-      <c r="B356"/>
-      <c r="C356"/>
-    </row>
-    <row r="357" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A357"/>
-      <c r="B357"/>
-      <c r="C357"/>
-    </row>
-    <row r="358" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A358"/>
-      <c r="B358"/>
-      <c r="C358"/>
-    </row>
-    <row r="359" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A359"/>
-      <c r="B359"/>
-      <c r="C359"/>
-    </row>
-    <row r="360" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A360"/>
-      <c r="B360"/>
-      <c r="C360"/>
-    </row>
-    <row r="361" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A361"/>
-      <c r="B361"/>
-      <c r="C361"/>
-    </row>
-    <row r="362" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A362"/>
-      <c r="B362"/>
-      <c r="C362"/>
-    </row>
-    <row r="363" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A363"/>
-      <c r="B363"/>
-      <c r="C363"/>
-    </row>
-    <row r="364" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A364"/>
-      <c r="B364"/>
-      <c r="C364"/>
-    </row>
-    <row r="365" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A365"/>
-      <c r="B365"/>
-      <c r="C365"/>
-    </row>
-    <row r="366" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A366"/>
-      <c r="B366"/>
-      <c r="C366"/>
-    </row>
-    <row r="367" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A367"/>
-      <c r="B367"/>
-      <c r="C367"/>
-    </row>
-    <row r="368" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A368"/>
-      <c r="B368"/>
-      <c r="C368"/>
-    </row>
-    <row r="369" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A369"/>
-      <c r="B369"/>
-      <c r="C369"/>
-    </row>
-    <row r="370" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A370"/>
-      <c r="B370"/>
-      <c r="C370"/>
-    </row>
-    <row r="371" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A371"/>
-      <c r="B371"/>
-      <c r="C371"/>
-    </row>
-    <row r="372" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A372"/>
-      <c r="B372"/>
-      <c r="C372"/>
-    </row>
-    <row r="373" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A373"/>
-      <c r="B373"/>
-      <c r="C373"/>
-    </row>
-    <row r="374" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A374"/>
-      <c r="B374"/>
-      <c r="C374"/>
-    </row>
-    <row r="375" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A375"/>
-      <c r="B375"/>
-      <c r="C375"/>
-    </row>
-    <row r="376" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A376"/>
-      <c r="B376"/>
-      <c r="C376"/>
-    </row>
-    <row r="377" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A377"/>
-      <c r="B377"/>
-      <c r="C377"/>
-    </row>
-    <row r="378" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A378"/>
-      <c r="B378"/>
-      <c r="C378"/>
-    </row>
-    <row r="379" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A379"/>
-      <c r="B379"/>
-      <c r="C379"/>
-    </row>
-    <row r="380" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A380"/>
-      <c r="B380"/>
-      <c r="C380"/>
-    </row>
-    <row r="381" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A381"/>
-      <c r="B381"/>
-      <c r="C381"/>
-    </row>
-    <row r="382" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A382"/>
-      <c r="B382"/>
-      <c r="C382"/>
-    </row>
-    <row r="383" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A383"/>
-      <c r="B383"/>
-      <c r="C383"/>
-    </row>
-    <row r="384" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A384"/>
-      <c r="B384"/>
-      <c r="C384"/>
-    </row>
-    <row r="385" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A385"/>
-      <c r="B385"/>
-      <c r="C385"/>
-    </row>
-    <row r="386" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A386"/>
-      <c r="B386"/>
-      <c r="C386"/>
-    </row>
-    <row r="387" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A387"/>
-      <c r="B387"/>
-      <c r="C387"/>
-    </row>
-    <row r="388" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A388"/>
-      <c r="B388"/>
-      <c r="C388"/>
-    </row>
-    <row r="389" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A389"/>
-      <c r="B389"/>
-      <c r="C389"/>
-    </row>
-    <row r="390" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A390"/>
-      <c r="B390"/>
-      <c r="C390"/>
-    </row>
-    <row r="391" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A391"/>
-      <c r="B391"/>
-      <c r="C391"/>
-    </row>
-    <row r="392" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A392"/>
-      <c r="B392"/>
-      <c r="C392"/>
-    </row>
-    <row r="393" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A393"/>
-      <c r="B393"/>
-      <c r="C393"/>
-    </row>
-    <row r="394" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A394"/>
-      <c r="B394"/>
-      <c r="C394"/>
-    </row>
-    <row r="395" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A395"/>
-      <c r="B395"/>
-      <c r="C395"/>
-    </row>
-    <row r="396" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A396"/>
-      <c r="B396"/>
-      <c r="C396"/>
-    </row>
-    <row r="397" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A397"/>
-      <c r="B397"/>
-      <c r="C397"/>
-    </row>
-    <row r="398" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A398"/>
-      <c r="B398"/>
-      <c r="C398"/>
-    </row>
-    <row r="399" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A399"/>
-      <c r="B399"/>
-      <c r="C399"/>
-    </row>
-    <row r="400" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A400"/>
-      <c r="B400"/>
-      <c r="C400"/>
-    </row>
-    <row r="401" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A401"/>
-      <c r="B401"/>
-      <c r="C401"/>
-    </row>
-    <row r="402" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A402"/>
-      <c r="B402"/>
-      <c r="C402"/>
-    </row>
-    <row r="403" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A403"/>
-      <c r="B403"/>
-      <c r="C403"/>
-    </row>
-    <row r="404" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A404"/>
-      <c r="B404"/>
-      <c r="C404"/>
-    </row>
-    <row r="405" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A405"/>
-      <c r="B405"/>
-      <c r="C405"/>
-    </row>
-    <row r="406" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A406"/>
-      <c r="B406"/>
-      <c r="C406"/>
-    </row>
-    <row r="407" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A407"/>
-      <c r="B407"/>
-      <c r="C407"/>
-    </row>
-    <row r="408" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A408"/>
-      <c r="B408"/>
-      <c r="C408"/>
-    </row>
-    <row r="409" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A409"/>
-      <c r="B409"/>
-      <c r="C409"/>
-    </row>
-    <row r="410" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A410"/>
-      <c r="B410"/>
-      <c r="C410"/>
-    </row>
-    <row r="411" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A411"/>
-      <c r="B411"/>
-      <c r="C411"/>
-    </row>
-    <row r="412" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A412"/>
-      <c r="B412"/>
-      <c r="C412"/>
-    </row>
-    <row r="413" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A413"/>
-      <c r="B413"/>
-      <c r="C413"/>
-    </row>
-    <row r="414" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A414"/>
-      <c r="B414"/>
-      <c r="C414"/>
-    </row>
-    <row r="415" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A415"/>
-      <c r="B415"/>
-      <c r="C415"/>
-    </row>
-    <row r="416" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A416"/>
-      <c r="B416"/>
-      <c r="C416"/>
-    </row>
-    <row r="417" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A417"/>
-      <c r="B417"/>
-      <c r="C417"/>
-    </row>
-    <row r="418" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A418"/>
-      <c r="B418"/>
-      <c r="C418"/>
-    </row>
-    <row r="419" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A419"/>
-      <c r="B419"/>
-      <c r="C419"/>
-    </row>
-    <row r="420" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A420"/>
-      <c r="B420"/>
-      <c r="C420"/>
-    </row>
-    <row r="421" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A421"/>
-      <c r="B421"/>
-      <c r="C421"/>
-    </row>
-    <row r="422" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A422"/>
-      <c r="B422"/>
-      <c r="C422"/>
-    </row>
-    <row r="423" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A423"/>
-      <c r="B423"/>
-      <c r="C423"/>
-    </row>
-    <row r="424" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A424"/>
-      <c r="B424"/>
-      <c r="C424"/>
-    </row>
-    <row r="425" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A425"/>
-      <c r="B425"/>
-      <c r="C425"/>
-    </row>
-    <row r="426" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A426"/>
-      <c r="B426"/>
-      <c r="C426"/>
-    </row>
-    <row r="427" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A427"/>
-      <c r="B427"/>
-      <c r="C427"/>
-    </row>
-    <row r="428" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A428"/>
-      <c r="B428"/>
-      <c r="C428"/>
-    </row>
-    <row r="429" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A429"/>
-      <c r="B429"/>
-      <c r="C429"/>
-    </row>
-    <row r="430" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A430"/>
-      <c r="B430"/>
-      <c r="C430"/>
-    </row>
-    <row r="431" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A431"/>
-      <c r="B431"/>
-      <c r="C431"/>
-    </row>
-    <row r="432" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A432"/>
-      <c r="B432"/>
-      <c r="C432"/>
-    </row>
-    <row r="433" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A433"/>
-      <c r="B433"/>
-      <c r="C433"/>
-    </row>
-    <row r="434" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A434"/>
-      <c r="B434"/>
-      <c r="C434"/>
-    </row>
-    <row r="435" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A435"/>
-      <c r="B435"/>
-      <c r="C435"/>
-    </row>
-    <row r="436" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A436"/>
-      <c r="B436"/>
-      <c r="C436"/>
-    </row>
-    <row r="437" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A437"/>
-      <c r="B437"/>
-      <c r="C437"/>
-    </row>
-    <row r="438" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A438"/>
-      <c r="B438"/>
-      <c r="C438"/>
-    </row>
-    <row r="439" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A439"/>
-      <c r="B439"/>
-      <c r="C439"/>
-    </row>
-    <row r="440" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A440"/>
-      <c r="B440"/>
-      <c r="C440"/>
-    </row>
-    <row r="441" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A441"/>
-      <c r="B441"/>
-      <c r="C441"/>
-    </row>
-    <row r="442" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A442"/>
-      <c r="B442"/>
-      <c r="C442"/>
-    </row>
-    <row r="443" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A443"/>
-      <c r="B443"/>
-      <c r="C443"/>
-    </row>
-    <row r="444" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A444"/>
-      <c r="B444"/>
-      <c r="C444"/>
-    </row>
-    <row r="445" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A445"/>
-      <c r="B445"/>
-      <c r="C445"/>
-    </row>
-    <row r="446" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A446"/>
-      <c r="B446"/>
-      <c r="C446"/>
-    </row>
-    <row r="447" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A447"/>
-      <c r="B447"/>
-      <c r="C447"/>
-    </row>
-    <row r="448" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A448"/>
-      <c r="B448"/>
-      <c r="C448"/>
-    </row>
-    <row r="449" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A449"/>
-      <c r="B449"/>
-      <c r="C449"/>
-    </row>
-    <row r="450" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A450"/>
-      <c r="B450"/>
-      <c r="C450"/>
-    </row>
-    <row r="451" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A451"/>
-      <c r="B451"/>
-      <c r="C451"/>
-    </row>
-    <row r="452" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A452"/>
-      <c r="B452"/>
-      <c r="C452"/>
-    </row>
-    <row r="453" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A453"/>
-      <c r="B453"/>
-      <c r="C453"/>
-    </row>
-    <row r="454" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A454"/>
-      <c r="B454"/>
-      <c r="C454"/>
-    </row>
-    <row r="455" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A455"/>
-      <c r="B455"/>
-      <c r="C455"/>
-    </row>
-    <row r="456" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A456"/>
-      <c r="B456"/>
-      <c r="C456"/>
-    </row>
-    <row r="457" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A457"/>
-      <c r="B457"/>
-      <c r="C457"/>
-    </row>
-    <row r="458" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A458"/>
-      <c r="B458"/>
-      <c r="C458"/>
-    </row>
-    <row r="459" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A459"/>
-      <c r="B459"/>
-      <c r="C459"/>
-    </row>
-    <row r="460" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A460"/>
-      <c r="B460"/>
-      <c r="C460"/>
-    </row>
-    <row r="461" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A461"/>
-      <c r="B461"/>
-      <c r="C461"/>
-    </row>
-    <row r="462" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A462"/>
-      <c r="B462"/>
-      <c r="C462"/>
-    </row>
-    <row r="463" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A463"/>
-      <c r="B463"/>
-      <c r="C463"/>
-    </row>
-    <row r="464" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A464"/>
-      <c r="B464"/>
-      <c r="C464"/>
-    </row>
-    <row r="465" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A465"/>
-      <c r="B465"/>
-      <c r="C465"/>
-    </row>
-    <row r="466" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A466"/>
-      <c r="B466"/>
-      <c r="C466"/>
-    </row>
-    <row r="467" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A467"/>
-      <c r="B467"/>
-      <c r="C467"/>
-    </row>
-    <row r="468" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A468"/>
-      <c r="B468"/>
-      <c r="C468"/>
-    </row>
-    <row r="469" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A469"/>
-      <c r="B469"/>
-      <c r="C469"/>
-    </row>
-    <row r="470" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A470"/>
-      <c r="B470"/>
-      <c r="C470"/>
-    </row>
-    <row r="471" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A471"/>
-      <c r="B471"/>
-      <c r="C471"/>
-    </row>
-    <row r="472" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A472"/>
-      <c r="B472"/>
-      <c r="C472"/>
-    </row>
-    <row r="473" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A473"/>
-      <c r="B473"/>
-      <c r="C473"/>
-    </row>
-    <row r="474" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A474"/>
-      <c r="B474"/>
-      <c r="C474"/>
-    </row>
+    <row r="241" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="242" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="243" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="244" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="245" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="246" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="247" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="248" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="249" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="250" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="251" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="252" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="253" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="254" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="255" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="256" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="257" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="258" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="259" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="260" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="261" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="262" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="263" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="264" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="265" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="266" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="267" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="268" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="269" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="270" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="271" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="272" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="273" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="274" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="275" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="276" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="277" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="278" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="279" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="280" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="281" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="282" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="283" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="284" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="285" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="286" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="287" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="288" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="289" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="290" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="291" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="292" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="293" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="294" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="295" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="296" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="297" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="298" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="299" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="300" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="301" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="302" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="303" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="304" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="305" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="306" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="307" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="308" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="309" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="310" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="311" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="312" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="313" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="314" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="315" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="316" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="317" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="318" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="319" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="320" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="321" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="322" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="323" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="324" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="325" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="326" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="327" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="328" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="329" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="330" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="331" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="332" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="333" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="334" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="335" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="336" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="337" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="338" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="339" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="340" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="341" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="342" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="343" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="344" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="345" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="346" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="347" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="348" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="349" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="350" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="351" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="352" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="353" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="354" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="355" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="356" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="357" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="358" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="359" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="360" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="361" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="362" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="363" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="364" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="365" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="366" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="367" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="368" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="369" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="370" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="371" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="372" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="373" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="374" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="375" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="376" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="377" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="378" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="379" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="380" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="381" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="382" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="383" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="384" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="385" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="386" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="387" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="388" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="389" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="390" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="391" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="392" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="393" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="394" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="395" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="396" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="397" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="398" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="399" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="400" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="401" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="402" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="403" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="404" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="405" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="406" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="407" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="408" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="409" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="410" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="411" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="412" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="413" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="414" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="415" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="416" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="417" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="418" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="419" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="420" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="421" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="422" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="423" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="424" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="425" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="426" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="427" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="428" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="429" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="430" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="431" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="432" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="433" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="434" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="435" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="436" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="437" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="438" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="439" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="440" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="441" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="442" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="443" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="444" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="445" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="446" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="447" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="448" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="449" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="450" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="451" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="452" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="453" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="454" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="455" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="456" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="457" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="458" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="459" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="460" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="461" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="462" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="463" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="464" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="465" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="466" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="467" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="468" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="469" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="470" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="471" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="472" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="473" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="474" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>